<commit_message>
fix year as float
</commit_message>
<xml_diff>
--- a/data_wrangling_2/raw_data/data_ticker.xlsx
+++ b/data_wrangling_2/raw_data/data_ticker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christineshearer/Desktop/workspace/Phaseout-dashboard/data_wrangling_2/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C9B50A-20EE-EE49-A477-997D457367F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342199F2-261C-834A-BF72-DCB8CBDD4687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="44800" windowHeight="23000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,9 +377,6 @@
     <t>Zimbabwe</t>
   </si>
   <si>
-    <t>Country/Area</t>
-  </si>
-  <si>
     <t>Pledged coal phaseout year</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -731,23 +731,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="3"/>
@@ -780,7 +780,7 @@
         <v>2040</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D2" s="8">
         <v>2126</v>
@@ -808,7 +808,7 @@
         <v>2040</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="8">
         <v>1968</v>
@@ -822,7 +822,7 @@
         <v>2030</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="8">
         <v>97</v>
@@ -836,7 +836,7 @@
         <v>2030</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D6" s="8">
         <v>443</v>
@@ -850,7 +850,7 @@
         <v>2040</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="8">
         <v>1472</v>
@@ -864,7 +864,7 @@
         <v>2040</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -878,7 +878,7 @@
         <v>2040</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="9">
         <v>0.495</v>
@@ -892,7 +892,7 @@
         <v>2030</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10" s="9">
         <v>22.402999999999999</v>
@@ -920,7 +920,7 @@
         <v>2040</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="9">
         <v>5.4349999999999996</v>
@@ -934,7 +934,7 @@
         <v>2040</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>2030</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="9">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>2040</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D15" s="9">
         <v>2.09</v>
@@ -976,7 +976,7 @@
         <v>2040</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="9">
         <v>0.73199999999999998</v>
@@ -990,7 +990,7 @@
         <v>2040</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" s="9">
         <v>3.177</v>
@@ -1004,7 +1004,7 @@
         <v>2040</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="9">
         <v>0.22</v>
@@ -1032,7 +1032,7 @@
         <v>2040</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" s="9">
         <v>1.4550000000000001</v>
@@ -1074,7 +1074,7 @@
         <v>2040</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D23" s="9">
         <v>1147.231</v>
@@ -1158,7 +1158,7 @@
         <v>2040</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D29" s="9">
         <v>1.198</v>
@@ -1172,7 +1172,7 @@
         <v>2040</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" s="9">
         <v>0</v>
@@ -1186,7 +1186,7 @@
         <v>2040</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D31" s="9">
         <v>1.0640000000000001</v>
@@ -1214,7 +1214,7 @@
         <v>2040</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" s="9">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>2040</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="9">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>2040</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D35" s="9">
         <v>0</v>
@@ -1284,7 +1284,7 @@
         <v>2040</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D38" s="9">
         <v>0</v>
@@ -1312,7 +1312,7 @@
         <v>2040</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D40" s="9">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>2040</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42" s="9">
         <v>6.4000000000000001E-2</v>
@@ -1354,7 +1354,7 @@
         <v>2040</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="9">
         <v>0.439</v>
@@ -1368,7 +1368,7 @@
         <v>2040</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D44" s="9">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>2040</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D45" s="9">
         <v>0.105</v>
@@ -1424,7 +1424,7 @@
         <v>2040</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="9">
         <v>239.64520000000002</v>
@@ -1438,7 +1438,7 @@
         <v>2040</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D49" s="9">
         <v>52.316600000000001</v>
@@ -1452,7 +1452,7 @@
         <v>2040</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D50" s="9">
         <v>0</v>
@@ -1508,7 +1508,7 @@
         <v>2040</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D54" s="9">
         <v>0</v>
@@ -1522,7 +1522,7 @@
         <v>2030</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D55" s="9">
         <v>54.750999999999998</v>
@@ -1536,7 +1536,7 @@
         <v>2040</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D56" s="9">
         <v>12.976000000000001</v>
@@ -1550,7 +1550,7 @@
         <v>2040</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D57" s="9">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>2040</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D59" s="9">
         <v>0.81299999999999994</v>
@@ -1592,7 +1592,7 @@
         <v>2040</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D60" s="9">
         <v>1.8779999999999999</v>
@@ -1606,7 +1606,7 @@
         <v>2030</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D61" s="9">
         <v>0</v>
@@ -1620,7 +1620,7 @@
         <v>2040</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D62" s="9">
         <v>0.12</v>
@@ -1634,7 +1634,7 @@
         <v>2040</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D63" s="9">
         <v>0</v>
@@ -1648,7 +1648,7 @@
         <v>2040</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D64" s="9">
         <v>13.28</v>
@@ -1676,7 +1676,7 @@
         <v>2030</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D66" s="9">
         <v>5.3780000000000001</v>
@@ -1690,7 +1690,7 @@
         <v>2040</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D67" s="9">
         <v>0</v>
@@ -1704,7 +1704,7 @@
         <v>2040</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" s="9">
         <v>0.995</v>
@@ -1732,7 +1732,7 @@
         <v>2040</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D70" s="9">
         <v>4.0919999999999996</v>
@@ -1746,7 +1746,7 @@
         <v>2040</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D71" s="9">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>2040</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D73" s="9">
         <v>0.12</v>
@@ -1802,7 +1802,7 @@
         <v>2040</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D75" s="9">
         <v>0.37</v>
@@ -1830,7 +1830,7 @@
         <v>2040</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="9">
         <v>0</v>
@@ -1844,7 +1844,7 @@
         <v>2040</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D78" s="9">
         <v>0.28449999999999998</v>
@@ -1858,7 +1858,7 @@
         <v>2040</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D79" s="9">
         <v>3.25</v>
@@ -1886,7 +1886,7 @@
         <v>2040</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D81" s="9">
         <v>0</v>
@@ -1900,7 +1900,7 @@
         <v>2040</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D82" s="9">
         <v>7.6379999999999999</v>
@@ -1928,7 +1928,7 @@
         <v>2040</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D84" s="9">
         <v>0</v>
@@ -1942,7 +1942,7 @@
         <v>2040</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D85" s="9">
         <v>0</v>
@@ -1956,7 +1956,7 @@
         <v>2040</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D86" s="9">
         <v>12.2324</v>
@@ -2012,7 +2012,7 @@
         <v>2040</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D90" s="9">
         <v>37.811099999999996</v>
@@ -2026,7 +2026,7 @@
         <v>2040</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D91" s="9">
         <v>0.155</v>
@@ -2082,7 +2082,7 @@
         <v>2040</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D95" s="9">
         <v>44.2241</v>
@@ -2138,7 +2138,7 @@
         <v>2040</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D99" s="9">
         <v>0</v>
@@ -2152,7 +2152,7 @@
         <v>2030</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D100" s="9">
         <v>0</v>
@@ -2166,7 +2166,7 @@
         <v>2040</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D101" s="9">
         <v>0</v>
@@ -2180,7 +2180,7 @@
         <v>2040</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D102" s="9">
         <v>19.155999999999999</v>
@@ -2194,7 +2194,7 @@
         <v>2040</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D103" s="9">
         <v>0.4</v>
@@ -2208,7 +2208,7 @@
         <v>2040</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D104" s="9">
         <v>0</v>
@@ -2222,7 +2222,7 @@
         <v>2040</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D105" s="9">
         <v>6.1379999999999999</v>
@@ -2236,7 +2236,7 @@
         <v>2030</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D106" s="9">
         <v>20.473200000000002</v>
@@ -2264,7 +2264,7 @@
         <v>2040</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D108" s="9">
         <v>0</v>
@@ -2306,7 +2306,7 @@
         <v>2040</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D111" s="9">
         <v>2.4929999999999999</v>
@@ -2320,7 +2320,7 @@
         <v>2040</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D112" s="9">
         <v>0</v>
@@ -2334,7 +2334,7 @@
         <v>2040</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D113" s="9">
         <v>27.239000000000001</v>
@@ -2348,7 +2348,7 @@
         <v>2040</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D114" s="9">
         <v>0.33</v>
@@ -2362,7 +2362,7 @@
         <v>2040</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D115" s="9">
         <v>1.67</v>

</xml_diff>

<commit_message>
gap in ambition labels
</commit_message>
<xml_diff>
--- a/data_wrangling_2/raw_data/data_ticker.xlsx
+++ b/data_wrangling_2/raw_data/data_ticker.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>2125.5271</v>
+        <v>2158.223</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>295.9937</v>
+        <v>300.0136</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
-        <v>1968.1992</v>
+        <v>1981.5681</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +508,7 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
-        <v>97.4918</v>
+        <v>102.1748</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
-        <v>442.9242</v>
+        <v>448.1091</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +536,7 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
-        <v>1472.0884</v>
+        <v>1478.9624</v>
       </c>
     </row>
     <row r="8">
@@ -578,7 +578,7 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
-        <v>22.403</v>
+        <v>22.863</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +708,7 @@
         <v>2038</v>
       </c>
       <c r="D19" t="n">
-        <v>4.569</v>
+        <v>5.109</v>
       </c>
     </row>
     <row r="20">
@@ -738,7 +738,7 @@
         <v>2030</v>
       </c>
       <c r="D21" t="n">
-        <v>3.2308</v>
+        <v>3.3808</v>
       </c>
     </row>
     <row r="22">
@@ -768,7 +768,7 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
-        <v>1147.231</v>
+        <v>1151.116</v>
       </c>
     </row>
     <row r="24">
@@ -816,7 +816,7 @@
         <v>2033</v>
       </c>
       <c r="D26" t="n">
-        <v>0.217</v>
+        <v>0.342</v>
       </c>
     </row>
     <row r="27">
@@ -832,7 +832,7 @@
         <v>2033</v>
       </c>
       <c r="D27" t="n">
-        <v>7.4036</v>
+        <v>7.4586</v>
       </c>
     </row>
     <row r="28">
@@ -1010,7 +1010,7 @@
         <v>2030</v>
       </c>
       <c r="D39" t="n">
-        <v>32.4055</v>
+        <v>34.4975</v>
       </c>
     </row>
     <row r="40">
@@ -1112,7 +1112,7 @@
         <v>2035</v>
       </c>
       <c r="D46" t="n">
-        <v>5.76</v>
+        <v>6.109999999999999</v>
       </c>
     </row>
     <row r="47">
@@ -1128,7 +1128,7 @@
         <v>2029</v>
       </c>
       <c r="D47" t="n">
-        <v>0.884</v>
+        <v>1.134</v>
       </c>
     </row>
     <row r="48">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="n">
-        <v>239.6452</v>
+        <v>240.1642</v>
       </c>
     </row>
     <row r="49">
@@ -1218,7 +1218,7 @@
         <v>2027</v>
       </c>
       <c r="D53" t="n">
-        <v>5.19</v>
+        <v>6.166</v>
       </c>
     </row>
     <row r="54">
@@ -1246,7 +1246,7 @@
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
-        <v>54.751</v>
+        <v>55.36</v>
       </c>
     </row>
     <row r="56">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C56" t="inlineStr"/>
       <c r="D56" t="n">
-        <v>12.976</v>
+        <v>13.606</v>
       </c>
     </row>
     <row r="57">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="C67" t="inlineStr"/>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="68">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>3.25</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="80">
@@ -1638,7 +1638,7 @@
       </c>
       <c r="C82" t="inlineStr"/>
       <c r="D82" t="n">
-        <v>7.638</v>
+        <v>7.788</v>
       </c>
     </row>
     <row r="83">
@@ -1744,7 +1744,7 @@
         <v>2032</v>
       </c>
       <c r="D89" t="n">
-        <v>2.31</v>
+        <v>2.955</v>
       </c>
     </row>
     <row r="90">
@@ -1800,7 +1800,7 @@
         <v>2050</v>
       </c>
       <c r="D93" t="n">
-        <v>4.435</v>
+        <v>4.467</v>
       </c>
     </row>
     <row r="94">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="C96" t="inlineStr"/>
       <c r="D96" t="n">
-        <v>44.2241</v>
+        <v>46.6941</v>
       </c>
     </row>
     <row r="97">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C102" t="inlineStr"/>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="103">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="C107" t="inlineStr"/>
       <c r="D107" t="n">
-        <v>20.4732</v>
+        <v>20.8732</v>
       </c>
     </row>
     <row r="108">
@@ -2022,7 +2022,7 @@
         <v>2035</v>
       </c>
       <c r="D108" t="n">
-        <v>5.422</v>
+        <v>21.477</v>
       </c>
     </row>
     <row r="109">
@@ -2068,7 +2068,7 @@
         <v>2035</v>
       </c>
       <c r="D111" t="n">
-        <v>196.2154</v>
+        <v>196.4083</v>
       </c>
     </row>
     <row r="112">

</xml_diff>